<commit_message>
Team Meeting Attendance Sep 22,2021
</commit_message>
<xml_diff>
--- a/Admin/attendance-sheet.xlsx
+++ b/Admin/attendance-sheet.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="SPONSOR" sheetId="1" state="visible" r:id="rId2"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="16">
   <si>
     <t xml:space="preserve">Sponsor Meetings</t>
   </si>
@@ -500,7 +500,7 @@
   <dimension ref="A1:W15"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D11" activeCellId="0" sqref="D11"/>
+      <selection pane="topLeft" activeCell="D11" activeCellId="1" sqref="E11 D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.9921875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1055,8 +1055,8 @@
   </sheetPr>
   <dimension ref="A1:W15"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D11" activeCellId="0" sqref="D11"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E11" activeCellId="0" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.9921875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1134,7 +1134,9 @@
       <c r="D3" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="10"/>
+      <c r="E3" s="10" t="s">
+        <v>2</v>
+      </c>
       <c r="F3" s="10"/>
       <c r="G3" s="10"/>
       <c r="H3" s="10"/>
@@ -1166,7 +1168,9 @@
       <c r="D4" s="11" t="n">
         <v>15</v>
       </c>
-      <c r="E4" s="11"/>
+      <c r="E4" s="11" t="n">
+        <v>22</v>
+      </c>
       <c r="F4" s="11"/>
       <c r="G4" s="11"/>
       <c r="H4" s="11"/>
@@ -1199,7 +1203,9 @@
       <c r="D5" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="E5" s="14"/>
+      <c r="E5" s="14" t="s">
+        <v>6</v>
+      </c>
       <c r="F5" s="14"/>
       <c r="G5" s="14"/>
       <c r="H5" s="14"/>
@@ -1211,7 +1217,7 @@
       <c r="N5" s="14"/>
       <c r="O5" s="15" t="n">
         <f aca="false">COUNTA(C5:N5)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="P5" s="16" t="n">
         <f aca="false">O5/COUNTA($C$4:$N$4)</f>
@@ -1238,7 +1244,9 @@
       <c r="D6" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="E6" s="14"/>
+      <c r="E6" s="14" t="s">
+        <v>6</v>
+      </c>
       <c r="F6" s="14"/>
       <c r="G6" s="14"/>
       <c r="H6" s="14"/>
@@ -1250,7 +1258,7 @@
       <c r="N6" s="14"/>
       <c r="O6" s="15" t="n">
         <f aca="false">COUNTA(C6:N6)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="P6" s="16" t="n">
         <f aca="false">O6/COUNTA($C$4:$N$4)</f>
@@ -1277,7 +1285,9 @@
       <c r="D7" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="E7" s="14"/>
+      <c r="E7" s="14" t="s">
+        <v>6</v>
+      </c>
       <c r="F7" s="14"/>
       <c r="G7" s="14"/>
       <c r="H7" s="14"/>
@@ -1289,7 +1299,7 @@
       <c r="N7" s="14"/>
       <c r="O7" s="15" t="n">
         <f aca="false">COUNTA(C7:N7)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="P7" s="16" t="n">
         <f aca="false">O7/COUNTA($C$4:$N$4)</f>
@@ -1314,7 +1324,9 @@
       <c r="D8" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="E8" s="14"/>
+      <c r="E8" s="14" t="s">
+        <v>6</v>
+      </c>
       <c r="F8" s="14"/>
       <c r="G8" s="14"/>
       <c r="H8" s="14"/>
@@ -1326,7 +1338,7 @@
       <c r="N8" s="14"/>
       <c r="O8" s="15" t="n">
         <f aca="false">COUNTA(C8:N8)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="P8" s="16" t="n">
         <f aca="false">O8/COUNTA($C$4:$N$4)</f>
@@ -1367,7 +1379,7 @@
       </c>
       <c r="P9" s="16" t="n">
         <f aca="false">O9/COUNTA($C$4:$N$4)</f>
-        <v>1</v>
+        <v>0.666666666666667</v>
       </c>
       <c r="Q9" s="6"/>
       <c r="R9" s="6"/>
@@ -1388,7 +1400,9 @@
       <c r="D10" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="E10" s="14"/>
+      <c r="E10" s="14" t="s">
+        <v>6</v>
+      </c>
       <c r="F10" s="14"/>
       <c r="G10" s="14"/>
       <c r="H10" s="14"/>
@@ -1400,7 +1414,7 @@
       <c r="N10" s="14"/>
       <c r="O10" s="15" t="n">
         <f aca="false">COUNTA(C10:N10)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="P10" s="16" t="n">
         <f aca="false">O10/COUNTA($C$4:$N$4)</f>
@@ -1425,7 +1439,9 @@
       <c r="D11" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="E11" s="14"/>
+      <c r="E11" s="14" t="s">
+        <v>6</v>
+      </c>
       <c r="F11" s="14"/>
       <c r="G11" s="14"/>
       <c r="H11" s="14"/>
@@ -1437,7 +1453,7 @@
       <c r="N11" s="14"/>
       <c r="O11" s="15" t="n">
         <f aca="false">COUNTA(C11:N11)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="P11" s="16" t="n">
         <f aca="false">O11/COUNTA($C$4:$N$4)</f>
@@ -1487,7 +1503,7 @@
       </c>
       <c r="E13" s="24" t="n">
         <f aca="false">COUNTA(E5:E12)</f>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="F13" s="24" t="n">
         <f aca="false">COUNTA(F5:F12)</f>
@@ -1617,8 +1633,8 @@
   </sheetPr>
   <dimension ref="A1:W15"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D32" activeCellId="0" sqref="D32"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D32" activeCellId="1" sqref="E11 D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.9921875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
Attendance Oct 8, 2021
</commit_message>
<xml_diff>
--- a/Admin/attendance-sheet.xlsx
+++ b/Admin/attendance-sheet.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="SPONSOR" sheetId="1" state="visible" r:id="rId2"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="17">
   <si>
     <t xml:space="preserve">Sponsor Meetings</t>
   </si>
@@ -321,7 +321,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="28">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -375,7 +375,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="13" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -395,7 +395,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="4" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="13" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="15" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="11" fillId="4" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -428,10 +428,6 @@
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="4" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -519,7 +515,7 @@
   <dimension ref="A1:W15"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E4" activeCellId="0" sqref="E4"/>
+      <selection pane="topLeft" activeCell="B5" activeCellId="1" sqref="G6 B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.9921875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1096,8 +1092,8 @@
   </sheetPr>
   <dimension ref="A1:W15"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F11" activeCellId="0" sqref="F11"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G6" activeCellId="0" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.9921875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1181,7 +1177,9 @@
       <c r="F3" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="G3" s="10"/>
+      <c r="G3" s="10" t="s">
+        <v>3</v>
+      </c>
       <c r="H3" s="10"/>
       <c r="I3" s="10"/>
       <c r="J3" s="10"/>
@@ -1217,7 +1215,9 @@
       <c r="F4" s="11" t="n">
         <v>29</v>
       </c>
-      <c r="G4" s="11"/>
+      <c r="G4" s="11" t="n">
+        <v>8</v>
+      </c>
       <c r="H4" s="11"/>
       <c r="I4" s="11"/>
       <c r="J4" s="11"/>
@@ -1254,7 +1254,9 @@
       <c r="F5" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="G5" s="14"/>
+      <c r="G5" s="14" t="s">
+        <v>7</v>
+      </c>
       <c r="H5" s="14"/>
       <c r="I5" s="14"/>
       <c r="J5" s="14"/>
@@ -1264,7 +1266,7 @@
       <c r="N5" s="14"/>
       <c r="O5" s="15" t="n">
         <f aca="false">COUNTA(C5:N5)</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="P5" s="16" t="n">
         <f aca="false">O5/COUNTA($C$4:$N$4)</f>
@@ -1297,7 +1299,9 @@
       <c r="F6" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="G6" s="14"/>
+      <c r="G6" s="14" t="s">
+        <v>7</v>
+      </c>
       <c r="H6" s="14"/>
       <c r="I6" s="14"/>
       <c r="J6" s="14"/>
@@ -1307,7 +1311,7 @@
       <c r="N6" s="14"/>
       <c r="O6" s="15" t="n">
         <f aca="false">COUNTA(C6:N6)</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="P6" s="16" t="n">
         <f aca="false">O6/COUNTA($C$4:$N$4)</f>
@@ -1340,7 +1344,9 @@
       <c r="F7" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="G7" s="14"/>
+      <c r="G7" s="14" t="s">
+        <v>7</v>
+      </c>
       <c r="H7" s="14"/>
       <c r="I7" s="14"/>
       <c r="J7" s="14"/>
@@ -1350,7 +1356,7 @@
       <c r="N7" s="14"/>
       <c r="O7" s="15" t="n">
         <f aca="false">COUNTA(C7:N7)</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="P7" s="16" t="n">
         <f aca="false">O7/COUNTA($C$4:$N$4)</f>
@@ -1381,7 +1387,9 @@
       <c r="F8" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="G8" s="14"/>
+      <c r="G8" s="14" t="s">
+        <v>7</v>
+      </c>
       <c r="H8" s="14"/>
       <c r="I8" s="14"/>
       <c r="J8" s="14"/>
@@ -1391,7 +1399,7 @@
       <c r="N8" s="14"/>
       <c r="O8" s="15" t="n">
         <f aca="false">COUNTA(C8:N8)</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="P8" s="16" t="n">
         <f aca="false">O8/COUNTA($C$4:$N$4)</f>
@@ -1422,7 +1430,9 @@
       <c r="F9" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="G9" s="14"/>
+      <c r="G9" s="14" t="s">
+        <v>7</v>
+      </c>
       <c r="H9" s="14"/>
       <c r="I9" s="14"/>
       <c r="J9" s="14"/>
@@ -1432,7 +1442,7 @@
       <c r="N9" s="14"/>
       <c r="O9" s="15" t="n">
         <f aca="false">COUNTA(C9:N9)</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="P9" s="16" t="n">
         <f aca="false">O9/COUNTA($C$4:$N$4)</f>
@@ -1463,7 +1473,9 @@
       <c r="F10" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="G10" s="14"/>
+      <c r="G10" s="14" t="s">
+        <v>7</v>
+      </c>
       <c r="H10" s="14"/>
       <c r="I10" s="14"/>
       <c r="J10" s="14"/>
@@ -1473,7 +1485,7 @@
       <c r="N10" s="14"/>
       <c r="O10" s="15" t="n">
         <f aca="false">COUNTA(C10:N10)</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="P10" s="16" t="n">
         <f aca="false">O10/COUNTA($C$4:$N$4)</f>
@@ -1504,7 +1516,9 @@
       <c r="F11" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="G11" s="14"/>
+      <c r="G11" s="14" t="s">
+        <v>7</v>
+      </c>
       <c r="H11" s="14"/>
       <c r="I11" s="14"/>
       <c r="J11" s="14"/>
@@ -1514,7 +1528,7 @@
       <c r="N11" s="14"/>
       <c r="O11" s="15" t="n">
         <f aca="false">COUNTA(C11:N11)</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="P11" s="16" t="n">
         <f aca="false">O11/COUNTA($C$4:$N$4)</f>
@@ -1572,7 +1586,7 @@
       </c>
       <c r="G13" s="24" t="n">
         <f aca="false">COUNTA(G5:G12)</f>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="H13" s="24" t="n">
         <f aca="false">COUNTA(H5:H12)</f>
@@ -1694,8 +1708,8 @@
   </sheetPr>
   <dimension ref="A1:W15"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D10" activeCellId="0" sqref="D10"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D10" activeCellId="1" sqref="G6 D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.9921875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1829,7 +1843,7 @@
         <f aca="true">OFFSET(A5,-1,0,1,1)+1</f>
         <v>1</v>
       </c>
-      <c r="B5" s="27" t="s">
+      <c r="B5" s="13" t="s">
         <v>6</v>
       </c>
       <c r="C5" s="14" t="s">
@@ -1868,7 +1882,7 @@
         <f aca="true">OFFSET(A6,-1,0,1,1)+1</f>
         <v>2</v>
       </c>
-      <c r="B6" s="27" t="s">
+      <c r="B6" s="13" t="s">
         <v>8</v>
       </c>
       <c r="C6" s="14" t="s">
@@ -1907,7 +1921,7 @@
         <f aca="true">OFFSET(A7,-1,0,1,1)+1</f>
         <v>3</v>
       </c>
-      <c r="B7" s="27" t="s">
+      <c r="B7" s="13" t="s">
         <v>9</v>
       </c>
       <c r="C7" s="14" t="s">
@@ -1944,7 +1958,7 @@
         <f aca="true">OFFSET(A8,-1,0,1,1)+1</f>
         <v>4</v>
       </c>
-      <c r="B8" s="27" t="s">
+      <c r="B8" s="13" t="s">
         <v>10</v>
       </c>
       <c r="C8" s="14" t="s">
@@ -1981,7 +1995,7 @@
         <f aca="true">OFFSET(A9,-1,0,1,1)+1</f>
         <v>5</v>
       </c>
-      <c r="B9" s="27" t="s">
+      <c r="B9" s="13" t="s">
         <v>11</v>
       </c>
       <c r="C9" s="14"/>
@@ -2016,7 +2030,7 @@
         <f aca="true">OFFSET(A10,-1,0,1,1)+1</f>
         <v>6</v>
       </c>
-      <c r="B10" s="27" t="s">
+      <c r="B10" s="13" t="s">
         <v>12</v>
       </c>
       <c r="C10" s="14" t="s">
@@ -2051,7 +2065,7 @@
         <f aca="true">OFFSET(A11,-1,0,1,1)+1</f>
         <v>7</v>
       </c>
-      <c r="B11" s="27" t="s">
+      <c r="B11" s="13" t="s">
         <v>13</v>
       </c>
       <c r="C11" s="14" t="s">
@@ -2085,7 +2099,7 @@
     </row>
     <row r="12" s="7" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="17"/>
-      <c r="B12" s="28"/>
+      <c r="B12" s="27"/>
       <c r="C12" s="19"/>
       <c r="D12" s="19"/>
       <c r="E12" s="19"/>

</xml_diff>

<commit_message>
Plus Ara who showed up late
</commit_message>
<xml_diff>
--- a/Admin/attendance-sheet.xlsx
+++ b/Admin/attendance-sheet.xlsx
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="18">
   <si>
     <t xml:space="preserve">Sponsor Meetings</t>
   </si>
@@ -518,7 +518,7 @@
   <dimension ref="A1:W15"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F11" activeCellId="1" sqref="F10 F11"/>
+      <selection pane="topLeft" activeCell="F11" activeCellId="1" sqref="F5 F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.9921875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1114,7 +1114,7 @@
   <dimension ref="A1:W15"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J4" activeCellId="2" sqref="F10 F11 J4"/>
+      <selection pane="topLeft" activeCell="J4" activeCellId="1" sqref="F5 J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.9921875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1768,7 +1768,7 @@
   <dimension ref="A1:W15"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F11" activeCellId="1" sqref="F10 F11"/>
+      <selection pane="topLeft" activeCell="F5" activeCellId="0" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.9921875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1922,7 +1922,9 @@
       <c r="E5" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="F5" s="14"/>
+      <c r="F5" s="14" t="s">
+        <v>7</v>
+      </c>
       <c r="G5" s="14"/>
       <c r="H5" s="14"/>
       <c r="I5" s="14"/>
@@ -1933,11 +1935,11 @@
       <c r="N5" s="14"/>
       <c r="O5" s="15" t="n">
         <f aca="false">COUNTA(C5:N5)</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="P5" s="16" t="n">
         <f aca="false">O5/COUNTA($C$4:$N$4)</f>
-        <v>0.75</v>
+        <v>1</v>
       </c>
       <c r="Q5" s="5"/>
       <c r="R5" s="6"/>
@@ -2231,7 +2233,7 @@
       </c>
       <c r="F13" s="24" t="n">
         <f aca="false">COUNTA(F5:F12)</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G13" s="24" t="n">
         <f aca="false">COUNTA(G5:G12)</f>

</xml_diff>

<commit_message>
Gaby time sheets | ATTENDANCE UP TO DATE NOV 29
</commit_message>
<xml_diff>
--- a/Admin/attendance-sheet.xlsx
+++ b/Admin/attendance-sheet.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="SPONSOR" sheetId="1" state="visible" r:id="rId2"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="18">
   <si>
     <t xml:space="preserve">Sponsor Meetings</t>
   </si>
@@ -517,8 +517,8 @@
   </sheetPr>
   <dimension ref="A1:W15"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G10" activeCellId="0" sqref="G10"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H5" activeCellId="1" sqref="G11 H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.9921875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -605,7 +605,9 @@
       <c r="G3" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="H3" s="10"/>
+      <c r="H3" s="10" t="s">
+        <v>4</v>
+      </c>
       <c r="I3" s="10"/>
       <c r="J3" s="10"/>
       <c r="K3" s="10"/>
@@ -643,7 +645,9 @@
       <c r="G4" s="11" t="n">
         <v>8</v>
       </c>
-      <c r="H4" s="11"/>
+      <c r="H4" s="11" t="n">
+        <v>29</v>
+      </c>
       <c r="I4" s="11"/>
       <c r="J4" s="11"/>
       <c r="K4" s="11"/>
@@ -682,7 +686,9 @@
       <c r="G5" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="H5" s="14"/>
+      <c r="H5" s="14" t="s">
+        <v>8</v>
+      </c>
       <c r="I5" s="14"/>
       <c r="J5" s="14"/>
       <c r="K5" s="14"/>
@@ -691,7 +697,7 @@
       <c r="N5" s="14"/>
       <c r="O5" s="15" t="n">
         <f aca="false">COUNTA(C5:N5)</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="P5" s="16" t="n">
         <f aca="false">O5/COUNTA($C$4:$N$4)</f>
@@ -725,7 +731,9 @@
       <c r="G6" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="H6" s="14"/>
+      <c r="H6" s="14" t="s">
+        <v>8</v>
+      </c>
       <c r="I6" s="14"/>
       <c r="J6" s="14"/>
       <c r="K6" s="14"/>
@@ -734,11 +742,11 @@
       <c r="N6" s="14"/>
       <c r="O6" s="15" t="n">
         <f aca="false">COUNTA(C6:N6)</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="P6" s="16" t="n">
         <f aca="false">O6/COUNTA($C$4:$N$4)</f>
-        <v>0.8</v>
+        <v>0.833333333333333</v>
       </c>
       <c r="Q6" s="5"/>
       <c r="R6" s="6"/>
@@ -770,7 +778,9 @@
       <c r="G7" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="H7" s="14"/>
+      <c r="H7" s="14" t="s">
+        <v>8</v>
+      </c>
       <c r="I7" s="14"/>
       <c r="J7" s="14"/>
       <c r="K7" s="14"/>
@@ -779,7 +789,7 @@
       <c r="N7" s="14"/>
       <c r="O7" s="15" t="n">
         <f aca="false">COUNTA(C7:N7)</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="P7" s="16" t="n">
         <f aca="false">O7/COUNTA($C$4:$N$4)</f>
@@ -813,7 +823,9 @@
       <c r="G8" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="H8" s="14"/>
+      <c r="H8" s="14" t="s">
+        <v>8</v>
+      </c>
       <c r="I8" s="14"/>
       <c r="J8" s="14"/>
       <c r="K8" s="14"/>
@@ -822,7 +834,7 @@
       <c r="N8" s="14"/>
       <c r="O8" s="15" t="n">
         <f aca="false">COUNTA(C8:N8)</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="P8" s="16" t="n">
         <f aca="false">O8/COUNTA($C$4:$N$4)</f>
@@ -854,7 +866,9 @@
       <c r="G9" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="H9" s="14"/>
+      <c r="H9" s="14" t="s">
+        <v>8</v>
+      </c>
       <c r="I9" s="14"/>
       <c r="J9" s="14"/>
       <c r="K9" s="14"/>
@@ -863,11 +877,11 @@
       <c r="N9" s="14"/>
       <c r="O9" s="15" t="n">
         <f aca="false">COUNTA(C9:N9)</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="P9" s="16" t="n">
         <f aca="false">O9/COUNTA($C$4:$N$4)</f>
-        <v>0.8</v>
+        <v>0.833333333333333</v>
       </c>
       <c r="Q9" s="6"/>
       <c r="R9" s="6"/>
@@ -895,7 +909,9 @@
       <c r="G10" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="H10" s="14"/>
+      <c r="H10" s="14" t="s">
+        <v>8</v>
+      </c>
       <c r="I10" s="14"/>
       <c r="J10" s="14"/>
       <c r="K10" s="14"/>
@@ -904,11 +920,11 @@
       <c r="N10" s="14"/>
       <c r="O10" s="15" t="n">
         <f aca="false">COUNTA(C10:N10)</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="P10" s="16" t="n">
         <f aca="false">O10/COUNTA($C$4:$N$4)</f>
-        <v>0.8</v>
+        <v>0.833333333333333</v>
       </c>
       <c r="Q10" s="2"/>
       <c r="R10" s="6"/>
@@ -938,7 +954,9 @@
       <c r="G11" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="H11" s="14"/>
+      <c r="H11" s="14" t="s">
+        <v>8</v>
+      </c>
       <c r="I11" s="14"/>
       <c r="J11" s="14"/>
       <c r="K11" s="14"/>
@@ -947,7 +965,7 @@
       <c r="N11" s="14"/>
       <c r="O11" s="15" t="n">
         <f aca="false">COUNTA(C11:N11)</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="P11" s="16" t="n">
         <f aca="false">O11/COUNTA($C$4:$N$4)</f>
@@ -1009,7 +1027,7 @@
       </c>
       <c r="H13" s="24" t="n">
         <f aca="false">COUNTA(H5:H12)</f>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="I13" s="24" t="n">
         <f aca="false">COUNTA(I5:I12)</f>
@@ -1105,11 +1123,11 @@
       <formula1>"1,2,3,4,5,6,7,8,9,10,11,12,13,14,15,16,17,18,19,20,21,22,23,24,25,26,27,28,29,30,31"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="C5:D11 H5:N11" type="list">
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="C5:D11 I5:N11" type="list">
       <formula1>SPONSOR!checkbox</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="E5:G11" type="list">
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="E5:H11" type="list">
       <formula1>SPONSOR!checkbox</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -1132,7 +1150,7 @@
   <dimension ref="A1:W15"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="T6" activeCellId="1" sqref="G10 T6"/>
+      <selection pane="topLeft" activeCell="L5" activeCellId="1" sqref="G11 L5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.9921875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1231,7 +1249,9 @@
       <c r="K3" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="L3" s="10"/>
+      <c r="L3" s="10" t="s">
+        <v>4</v>
+      </c>
       <c r="M3" s="10"/>
       <c r="N3" s="10"/>
       <c r="O3" s="9" t="s">
@@ -1277,7 +1297,9 @@
       <c r="K4" s="11" t="n">
         <v>4</v>
       </c>
-      <c r="L4" s="11"/>
+      <c r="L4" s="11" t="n">
+        <v>19</v>
+      </c>
       <c r="M4" s="11"/>
       <c r="N4" s="11"/>
       <c r="O4" s="9"/>
@@ -1324,12 +1346,14 @@
       <c r="K5" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="L5" s="14"/>
+      <c r="L5" s="14" t="s">
+        <v>8</v>
+      </c>
       <c r="M5" s="14"/>
       <c r="N5" s="14"/>
       <c r="O5" s="15" t="n">
         <f aca="false">COUNTA(C5:N5)</f>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="P5" s="16" t="n">
         <f aca="false">O5/COUNTA($C$4:$N$4)</f>
@@ -1377,12 +1401,14 @@
       <c r="K6" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="L6" s="14"/>
+      <c r="L6" s="14" t="s">
+        <v>8</v>
+      </c>
       <c r="M6" s="14"/>
       <c r="N6" s="14"/>
       <c r="O6" s="15" t="n">
         <f aca="false">COUNTA(C6:N6)</f>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="P6" s="16" t="n">
         <f aca="false">O6/COUNTA($C$4:$N$4)</f>
@@ -1430,12 +1456,14 @@
       <c r="K7" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="L7" s="14"/>
+      <c r="L7" s="14" t="s">
+        <v>8</v>
+      </c>
       <c r="M7" s="14"/>
       <c r="N7" s="14"/>
       <c r="O7" s="15" t="n">
         <f aca="false">COUNTA(C7:N7)</f>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="P7" s="16" t="n">
         <f aca="false">O7/COUNTA($C$4:$N$4)</f>
@@ -1481,12 +1509,14 @@
       <c r="K8" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="L8" s="14"/>
+      <c r="L8" s="14" t="s">
+        <v>8</v>
+      </c>
       <c r="M8" s="14"/>
       <c r="N8" s="14"/>
       <c r="O8" s="15" t="n">
         <f aca="false">COUNTA(C8:N8)</f>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="P8" s="16" t="n">
         <f aca="false">O8/COUNTA($C$4:$N$4)</f>
@@ -1528,16 +1558,18 @@
       <c r="K9" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="L9" s="14"/>
+      <c r="L9" s="14" t="s">
+        <v>8</v>
+      </c>
       <c r="M9" s="14"/>
       <c r="N9" s="14"/>
       <c r="O9" s="15" t="n">
         <f aca="false">COUNTA(C9:N9)</f>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="P9" s="16" t="n">
         <f aca="false">O9/COUNTA($C$4:$N$4)</f>
-        <v>0.777777777777778</v>
+        <v>0.8</v>
       </c>
       <c r="Q9" s="6"/>
       <c r="R9" s="6"/>
@@ -1579,12 +1611,14 @@
       <c r="K10" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="L10" s="14"/>
+      <c r="L10" s="14" t="s">
+        <v>8</v>
+      </c>
       <c r="M10" s="14"/>
       <c r="N10" s="14"/>
       <c r="O10" s="15" t="n">
         <f aca="false">COUNTA(C10:N10)</f>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="P10" s="16" t="n">
         <f aca="false">O10/COUNTA($C$4:$N$4)</f>
@@ -1630,12 +1664,14 @@
       <c r="K11" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="L11" s="14"/>
+      <c r="L11" s="14" t="s">
+        <v>8</v>
+      </c>
       <c r="M11" s="14"/>
       <c r="N11" s="14"/>
       <c r="O11" s="15" t="n">
         <f aca="false">COUNTA(C11:N11)</f>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="P11" s="16" t="n">
         <f aca="false">O11/COUNTA($C$4:$N$4)</f>
@@ -1815,8 +1851,8 @@
   </sheetPr>
   <dimension ref="A1:W15"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F5" activeCellId="1" sqref="G10 F5"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G11" activeCellId="0" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.9921875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1900,7 +1936,9 @@
       <c r="F3" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="G3" s="10"/>
+      <c r="G3" s="10" t="s">
+        <v>4</v>
+      </c>
       <c r="H3" s="10"/>
       <c r="I3" s="10"/>
       <c r="J3" s="10"/>
@@ -1936,7 +1974,9 @@
       <c r="F4" s="11" t="n">
         <v>3</v>
       </c>
-      <c r="G4" s="11"/>
+      <c r="G4" s="11" t="n">
+        <v>17</v>
+      </c>
       <c r="H4" s="11"/>
       <c r="I4" s="11"/>
       <c r="J4" s="11"/>
@@ -1973,7 +2013,9 @@
       <c r="F5" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="G5" s="14"/>
+      <c r="G5" s="14" t="s">
+        <v>8</v>
+      </c>
       <c r="H5" s="14"/>
       <c r="I5" s="14"/>
       <c r="J5" s="14"/>
@@ -1983,7 +2025,7 @@
       <c r="N5" s="14"/>
       <c r="O5" s="15" t="n">
         <f aca="false">COUNTA(C5:N5)</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="P5" s="16" t="n">
         <f aca="false">O5/COUNTA($C$4:$N$4)</f>
@@ -2016,7 +2058,9 @@
       <c r="F6" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="G6" s="14"/>
+      <c r="G6" s="14" t="s">
+        <v>8</v>
+      </c>
       <c r="H6" s="14"/>
       <c r="I6" s="14"/>
       <c r="J6" s="14"/>
@@ -2026,7 +2070,7 @@
       <c r="N6" s="14"/>
       <c r="O6" s="15" t="n">
         <f aca="false">COUNTA(C6:N6)</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="P6" s="16" t="n">
         <f aca="false">O6/COUNTA($C$4:$N$4)</f>
@@ -2059,7 +2103,9 @@
       <c r="F7" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="G7" s="14"/>
+      <c r="G7" s="14" t="s">
+        <v>8</v>
+      </c>
       <c r="H7" s="14"/>
       <c r="I7" s="14"/>
       <c r="J7" s="14"/>
@@ -2069,7 +2115,7 @@
       <c r="N7" s="14"/>
       <c r="O7" s="15" t="n">
         <f aca="false">COUNTA(C7:N7)</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="P7" s="16" t="n">
         <f aca="false">O7/COUNTA($C$4:$N$4)</f>
@@ -2100,7 +2146,9 @@
       <c r="F8" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="G8" s="14"/>
+      <c r="G8" s="14" t="s">
+        <v>8</v>
+      </c>
       <c r="H8" s="14"/>
       <c r="I8" s="14"/>
       <c r="J8" s="14"/>
@@ -2110,7 +2158,7 @@
       <c r="N8" s="14"/>
       <c r="O8" s="15" t="n">
         <f aca="false">COUNTA(C8:N8)</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="P8" s="16" t="n">
         <f aca="false">O8/COUNTA($C$4:$N$4)</f>
@@ -2137,7 +2185,9 @@
         <v>8</v>
       </c>
       <c r="F9" s="14"/>
-      <c r="G9" s="14"/>
+      <c r="G9" s="14" t="s">
+        <v>8</v>
+      </c>
       <c r="H9" s="14"/>
       <c r="I9" s="14"/>
       <c r="J9" s="14"/>
@@ -2147,11 +2197,11 @@
       <c r="N9" s="14"/>
       <c r="O9" s="15" t="n">
         <f aca="false">COUNTA(C9:N9)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="P9" s="16" t="n">
         <f aca="false">O9/COUNTA($C$4:$N$4)</f>
-        <v>0.5</v>
+        <v>0.6</v>
       </c>
       <c r="Q9" s="6"/>
       <c r="R9" s="6"/>
@@ -2190,7 +2240,7 @@
       </c>
       <c r="P10" s="16" t="n">
         <f aca="false">O10/COUNTA($C$4:$N$4)</f>
-        <v>0.75</v>
+        <v>0.6</v>
       </c>
       <c r="Q10" s="2"/>
       <c r="R10" s="6"/>
@@ -2217,7 +2267,9 @@
       <c r="F11" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="G11" s="14"/>
+      <c r="G11" s="14" t="s">
+        <v>8</v>
+      </c>
       <c r="H11" s="14"/>
       <c r="I11" s="14"/>
       <c r="J11" s="14"/>
@@ -2227,7 +2279,7 @@
       <c r="N11" s="14"/>
       <c r="O11" s="15" t="n">
         <f aca="false">COUNTA(C11:N11)</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="P11" s="16" t="n">
         <f aca="false">O11/COUNTA($C$4:$N$4)</f>
@@ -2285,7 +2337,7 @@
       </c>
       <c r="G13" s="24" t="n">
         <f aca="false">COUNTA(G5:G12)</f>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="H13" s="24" t="n">
         <f aca="false">COUNTA(H5:H12)</f>

</xml_diff>